<commit_message>
added Poiji dependency to read ExcelData using POJO class
</commit_message>
<xml_diff>
--- a/src/test/resource/TestData/ExcelFiles/bookList.xlsx
+++ b/src/test/resource/TestData/ExcelFiles/bookList.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="ProgrammingBooks" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -211,12 +211,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -282,7 +282,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -292,12 +292,11 @@
       <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.66"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -402,7 +401,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>